<commit_message>
Creacion de seccion e-commerce
</commit_message>
<xml_diff>
--- a/resources/Template_carga_productos.xlsx
+++ b/resources/Template_carga_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\Ingenieria-de-Software-2024\Web-Generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231BEC41-DF6B-43D4-807A-D469CE5B31A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9971319-3E26-4D0B-A3F3-7BDB43DB1D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{89D1E6DB-E25C-42C1-B3F0-4230522B4015}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89D1E6DB-E25C-42C1-B3F0-4230522B4015}"/>
   </bookViews>
   <sheets>
     <sheet name="carga_productos" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t>Multimedia_1</t>
-  </si>
-  <si>
     <t>Multimedia_2</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Multimedia_4</t>
+  </si>
+  <si>
+    <t>Imagen_principal</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,16 +906,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor parcial a ReactGenerator
</commit_message>
<xml_diff>
--- a/resources/Template_carga_productos.xlsx
+++ b/resources/Template_carga_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\Ingenieria-de-Software-2024\Web-Generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9971319-3E26-4D0B-A3F3-7BDB43DB1D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB289F32-BB0A-4841-81B5-35F8B0B2B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89D1E6DB-E25C-42C1-B3F0-4230522B4015}"/>
+    <workbookView xWindow="6030" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{89D1E6DB-E25C-42C1-B3F0-4230522B4015}"/>
   </bookViews>
   <sheets>
     <sheet name="carga_productos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Cantidad</t>
   </si>
@@ -34,16 +34,10 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t>Multimedia_2</t>
+    <t>Imagen_principal</t>
   </si>
   <si>
-    <t>Multimedia_3</t>
-  </si>
-  <si>
-    <t>Multimedia_4</t>
-  </si>
-  <si>
-    <t>Imagen_principal</t>
+    <t>(La imagen debe ser un link)</t>
   </si>
 </sst>
 </file>
@@ -884,15 +878,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A131D288-CD17-4CC7-B9A5-1BFE29703CF3}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,16 +903,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
captura de productos con SKU
</commit_message>
<xml_diff>
--- a/resources/Template_carga_productos.xlsx
+++ b/resources/Template_carga_productos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27716"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\Ingenieria-de-Software-2024\Web-Generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB289F32-BB0A-4841-81B5-35F8B0B2B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE9C1FE-0430-450B-9B0B-353AFAE1A8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6030" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{89D1E6DB-E25C-42C1-B3F0-4230522B4015}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Cantidad</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>(La imagen debe ser un link)</t>
+  </si>
+  <si>
+    <t>SKU</t>
   </si>
 </sst>
 </file>
@@ -878,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A131D288-CD17-4CC7-B9A5-1BFE29703CF3}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,23 +892,26 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>